<commit_message>
tables of models edited
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="27560" yWindow="480" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -54,27 +54,6 @@
     <t>Estimated coefficient</t>
   </si>
   <si>
-    <t>p-value</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>0 ***</t>
-  </si>
-  <si>
-    <t>0.0415 *</t>
-  </si>
-  <si>
-    <t>0.019 *</t>
-  </si>
-  <si>
-    <t>0.0029 **</t>
-  </si>
-  <si>
-    <t>0.004 **</t>
-  </si>
-  <si>
     <t xml:space="preserve">(Intercept)      </t>
   </si>
   <si>
@@ -90,24 +69,6 @@
     <t xml:space="preserve">SiteOmicron           </t>
   </si>
   <si>
-    <t>0.0006 ***</t>
-  </si>
-  <si>
-    <t>1.18e-06 ***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.002 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.005 ** </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: * denotes  0.01&lt; p-value &lt; 0.05; ** denotes 0.001&lt; p-value &lt; 0.01; *** denotes p-value &lt; 0.001  </t>
-  </si>
-  <si>
-    <t>Table 2. Coefficients and p-values for the linear regression model of otters having access to water</t>
-  </si>
-  <si>
     <t xml:space="preserve">log(Trout)           </t>
   </si>
   <si>
@@ -129,69 +90,320 @@
     <t xml:space="preserve">SiteOmicron       </t>
   </si>
   <si>
-    <t>1.35e-07 ***</t>
-  </si>
-  <si>
-    <t>1.22e-06 ***</t>
-  </si>
-  <si>
-    <t>1.89e-06 ***</t>
-  </si>
-  <si>
     <t xml:space="preserve">log(Altitude)          </t>
   </si>
   <si>
     <t xml:space="preserve">log(Trout)            </t>
   </si>
   <si>
+    <t xml:space="preserve">log(Trout):OtterRO-255     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(Trout):OtterRO-918   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(Trout):OtterRO-255  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(Trout):OtterRO-599    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(Trout):OtterRO-859  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(Trout):OtterRO-918  </t>
+  </si>
+  <si>
+    <t>Standard error</t>
+  </si>
+  <si>
+    <r>
+      <t>0.121</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.009</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.565</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.419</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <t>Table 3. Coefficients and standard errors for the mixed effect model of otters having access to water</t>
+  </si>
+  <si>
+    <t>Table 4. Coefficients and standard errors for the mixed effect model of all otters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>0.003215 **</t>
-    </r>
-  </si>
-  <si>
+      <t>denotes that the variable is significant.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>denotes that the variable is significant.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.112</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.415</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.491</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.095</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <t>σe and σa denote the residual and standard deviation of the random intercept, correspondingly.</t>
+  </si>
+  <si>
+    <t>Table 2. Coefficients and standard errors for the mixed effect model of otters having access to amoeba</t>
+  </si>
+  <si>
+    <r>
+      <t>0.191</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.013</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.704</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.740</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.118</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <t>σe = 0.241; σa = 0.144</t>
+  </si>
+  <si>
+    <t>σe = 0.179; σa = 0.107</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">σe = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>0.0006 ***</t>
-    </r>
-  </si>
-  <si>
-    <t>Table 3. Coefficients and p-values for the linear regression model of all otters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-255     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-918   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-255  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-599    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-859  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">log(Trout):OtterRO-918  </t>
-  </si>
-  <si>
-    <t>σa = 0.107; σe = 0.179</t>
-  </si>
-  <si>
-    <t>Table 1. Estimates and p-values for the mixed effect model of otters having access to amoeba</t>
-  </si>
-  <si>
-    <t>N/A: not applicable</t>
+      <t xml:space="preserve">0.225; σa = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>0.134</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -201,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -263,6 +475,16 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -278,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -300,17 +522,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color theme="8" tint="0.39997558519241921"/>
@@ -357,7 +568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,8 +600,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,16 +655,13 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -458,8 +686,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -475,6 +707,16 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -490,6 +732,16 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -547,6 +799,15 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -556,11 +817,28 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -597,6 +875,38 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -612,46 +922,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <color rgb="FF000000"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
@@ -691,7 +962,6 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -724,24 +994,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color theme="1"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
@@ -759,31 +1011,31 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Variable" dataDxfId="14"/>
     <tableColumn id="2" name="Estimated coefficient" dataDxfId="13"/>
-    <tableColumn id="3" name="p-value" dataDxfId="12"/>
+    <tableColumn id="3" name="Standard error" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A15:C23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A15:C23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
   <autoFilter ref="A15:C23"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Variable" dataDxfId="7"/>
-    <tableColumn id="2" name="Estimated coefficient" dataDxfId="6"/>
-    <tableColumn id="3" name="p-value" dataDxfId="5"/>
+    <tableColumn id="1" name="Variable" dataDxfId="8"/>
+    <tableColumn id="2" name="Estimated coefficient" dataDxfId="7"/>
+    <tableColumn id="3" name="Standard error" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A29:C41" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A29:C41" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="10">
   <autoFilter ref="A29:C41"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Variable" dataDxfId="2"/>
-    <tableColumn id="2" name="Estimated coefficient" dataDxfId="1"/>
-    <tableColumn id="3" name="p-value" dataDxfId="0"/>
+    <tableColumn id="1" name="Variable" dataDxfId="12"/>
+    <tableColumn id="2" name="Estimated coefficient" dataDxfId="11"/>
+    <tableColumn id="3" name="Standard error" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1111,17 +1363,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1132,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5"/>
     </row>
@@ -1143,8 +1395,8 @@
       <c r="B2" s="8">
         <v>1.2310892</v>
       </c>
-      <c r="C2" s="8">
-        <v>0.1966</v>
+      <c r="C2" s="23">
+        <v>0.94089999999999996</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
@@ -1156,8 +1408,8 @@
       <c r="B3" s="8">
         <v>0.67094589999999998</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
+      <c r="C3" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="1"/>
@@ -1169,8 +1421,8 @@
       <c r="B4" s="8">
         <v>-3.2009999999999999E-3</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
+      <c r="C4" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="1"/>
@@ -1182,8 +1434,8 @@
       <c r="B5" s="8">
         <v>3.2570300000000003E-2</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
+      <c r="C5" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="1"/>
@@ -1195,8 +1447,8 @@
       <c r="B6" s="8">
         <v>-2.2263885999999999</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>12</v>
+      <c r="C6" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1"/>
@@ -1208,8 +1460,8 @@
       <c r="B7" s="8">
         <v>-6.2229399999999997E-2</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>12</v>
+      <c r="C7" s="8">
+        <v>0.64500000000000002</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="1"/>
@@ -1221,8 +1473,8 @@
       <c r="B8" s="8">
         <v>-1.026505</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>14</v>
+      <c r="C8" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="1"/>
@@ -1235,7 +1487,7 @@
         <v>1.070667</v>
       </c>
       <c r="C9" s="8">
-        <v>0.1232</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="1"/>
@@ -1248,36 +1500,35 @@
         <v>2.6529145000000001</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="10" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="18"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="13" t="s">
@@ -1286,281 +1537,304 @@
       <c r="B15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>-2.9049200000000002</v>
       </c>
-      <c r="C16" s="21">
-        <v>9.3757999999999994E-2</v>
-      </c>
+      <c r="C16" s="20">
+        <v>1.7076</v>
+      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="21">
+      <c r="A17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="20">
         <v>0.7</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>23</v>
-      </c>
+      <c r="C17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="21">
+      <c r="A18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="20">
         <v>4.1270000000000001E-2</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="20">
+        <v>3.70695</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="20">
+        <v>2.1071</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="20">
+        <v>-9.4420000000000004E-2</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0.121</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="21">
-        <v>3.70695</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="21">
-        <v>2.1071</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="B22" s="20">
+        <v>0.39084000000000002</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="21">
-        <v>-9.4420000000000004E-2</v>
-      </c>
-      <c r="C21" s="21">
-        <v>0.44010700000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="21">
-        <v>0.39084000000000002</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <v>0.13972999999999999</v>
       </c>
-      <c r="C23" s="21">
-        <v>0.18092900000000001</v>
+      <c r="C23" s="20">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
+      <c r="A24" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="A25" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="3"/>
+      <c r="C29" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="27"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="21">
+        <v>17</v>
+      </c>
+      <c r="B30" s="20">
         <v>3.8758000000000001E-2</v>
       </c>
-      <c r="C30" s="21">
-        <v>0.96942399999999995</v>
+      <c r="C30" s="20">
+        <v>1.0171867000000001</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="21">
+        <v>23</v>
+      </c>
+      <c r="B31" s="20">
         <v>0.692222</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>36</v>
+      <c r="C31" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="21">
+        <v>18</v>
+      </c>
+      <c r="B32" s="20">
         <v>4.4144000000000003E-2</v>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>38</v>
+      <c r="C32" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="21">
+        <v>19</v>
+      </c>
+      <c r="B33" s="20">
         <v>-2.7720980000000002</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>37</v>
+      <c r="C33" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="21">
+        <v>20</v>
+      </c>
+      <c r="B34" s="20">
         <v>0.90221899999999999</v>
       </c>
-      <c r="C34" s="21">
-        <v>7.7747999999999998E-2</v>
+      <c r="C34" s="20">
+        <v>0.54001049999999995</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="21">
+        <v>21</v>
+      </c>
+      <c r="B35" s="20">
         <v>-1.133151</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>41</v>
+      <c r="C35" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="21">
+        <v>22</v>
+      </c>
+      <c r="B36" s="20">
         <v>-0.74510399999999999</v>
       </c>
-      <c r="C36" s="21">
-        <v>5.9199000000000002E-2</v>
+      <c r="C36" s="20">
+        <v>0.43360789999999999</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="21">
+        <v>24</v>
+      </c>
+      <c r="B37" s="20">
         <v>-0.113951</v>
       </c>
-      <c r="C37" s="21">
-        <v>0.246</v>
+      <c r="C37" s="20">
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="21">
+        <v>27</v>
+      </c>
+      <c r="B38" s="20">
         <v>0.38614999999999999</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>42</v>
+      <c r="C38" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="21">
+        <v>28</v>
+      </c>
+      <c r="B39" s="20">
         <v>0.12881999999999999</v>
       </c>
-      <c r="C39" s="21">
-        <v>0.15814900000000001</v>
+      <c r="C39" s="20">
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="21">
+        <v>29</v>
+      </c>
+      <c r="B40" s="20">
         <v>7.8758999999999996E-2</v>
       </c>
-      <c r="C40" s="21">
-        <v>0.39560899999999999</v>
+      <c r="C40" s="20">
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="21">
+        <v>30</v>
+      </c>
+      <c r="B41" s="20">
         <v>0.14385000000000001</v>
       </c>
-      <c r="C41" s="21">
-        <v>0.13461699999999999</v>
-      </c>
-      <c r="D41" s="3"/>
+      <c r="C41" s="20">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
+      <c r="A42" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>